<commit_message>
refactor: move components that are used in Code Analysis
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\visualgo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860B6399-E9AE-4DC1-ADD0-74159A780299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577E2C28-8100-41AE-A608-E8E8BA72060F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10824" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14832" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Priority</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -91,7 +91,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>socket.io send pythoncode</t>
+    <t>AST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>separate modules</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>separate python running modules from editor.vue</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -453,11 +461,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.95" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -525,41 +533,52 @@
       <c r="C4" s="1">
         <v>1</v>
       </c>
+      <c r="D4" s="3">
+        <v>45423</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="1" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C9" s="1">
         <v>1</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D9" s="3">
         <v>45421</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="D9" s="3"/>
+    <row r="10" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D10" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>